<commit_message>
Test with dplyr import, and readr/readxl for read/write_data
</commit_message>
<xml_diff>
--- a/tests/testthat/xlsx.xlsx
+++ b/tests/testthat/xlsx.xlsx
@@ -1,25 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\reporttool\tests\testthat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13130" windowHeight="6110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
+  <calcPr calcId="0"/>
   <sheets>
     <sheet name="xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>mainentity</t>
   </si>
@@ -58,13 +51,23 @@
   </si>
   <si>
     <t>Å</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>#NAME?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -72,24 +75,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7DC6CC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,17 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,30 +393,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2"/>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -436,10 +425,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -447,9 +439,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -460,6 +455,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>